<commit_message>
update logic lieu used
</commit_message>
<xml_diff>
--- a/uploads/temp_otlieu.xlsx
+++ b/uploads/temp_otlieu.xlsx
@@ -561,11 +561,11 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>18:20</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="N2" t="n">
-        <v>8.83</v>
+        <v>8.5</v>
       </c>
       <c r="O2" t="inlineStr"/>
     </row>
@@ -756,7 +756,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>2.33</t>
+          <t>1.67</t>
         </is>
       </c>
       <c r="O5" t="inlineStr"/>

</xml_diff>

<commit_message>
report logic & export function
</commit_message>
<xml_diff>
--- a/uploads/temp_otlieu.xlsx
+++ b/uploads/temp_otlieu.xlsx
@@ -620,11 +620,11 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="N3" t="n">
-        <v>9.5</v>
+        <v>8.5</v>
       </c>
       <c r="O3" t="inlineStr"/>
     </row>

</xml_diff>

<commit_message>
attendance report logic still fixing
</commit_message>
<xml_diff>
--- a/uploads/temp_otlieu.xlsx
+++ b/uploads/temp_otlieu.xlsx
@@ -556,16 +556,16 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>08 : Minutes AM</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>06 : Minutes PM</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="N2" t="n">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="O2" t="inlineStr"/>
     </row>
@@ -615,16 +615,16 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>08 : Minutes AM</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>06 : Minutes PM</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="N3" t="n">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="O3" t="inlineStr"/>
     </row>
@@ -756,8 +756,10 @@
           <t>10:20</t>
         </is>
       </c>
-      <c r="N5" t="n">
-        <v>1.67</v>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>2.33</t>
+        </is>
       </c>
       <c r="O5" t="inlineStr"/>
     </row>
@@ -1463,7 +1465,7 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>2:</t>
+          <t>2</t>
         </is>
       </c>
       <c r="O16" t="inlineStr"/>

</xml_diff>